<commit_message>
feat: enhance supplier logo upload, refine config, migrate ro_consult (removed large dump files)
</commit_message>
<xml_diff>
--- a/data/area_atu.xlsx
+++ b/data/area_atu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sistemas_ia\SalesMasters\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B60184B-AF66-42E9-B096-DF22B2D431B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74FDC91-2226-46CC-9570-7D54BC2BEF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
   <si>
     <t>ATU_ID</t>
   </si>
@@ -34,103 +34,148 @@
     <t>GID</t>
   </si>
   <si>
-    <t>SEM ATUACAO</t>
-  </si>
-  <si>
     <t>AGRICOLA-TODAS</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>6611C245-49D3-4A52-BE9D-C1A517F59CE8</t>
+  </si>
+  <si>
     <t>AGRICOLA-AGRALE</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>FE16A6BC-3064-4B48-AF46-F8B507F5F26E</t>
+  </si>
+  <si>
     <t>AGRICOLA-CBT</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>F3120D45-18C9-4560-B2DD-51A93CC1C853</t>
+  </si>
+  <si>
     <t>AGRICOLA-JACTOR</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>4FD34704-0B19-4DEA-9A25-8C32B2F11A92</t>
+  </si>
+  <si>
     <t>AGRICOLA-JOHN DEERE</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>B68FDE8D-FB04-4591-A6E4-89B290CBB29F</t>
+  </si>
+  <si>
     <t>AGRICOLA-MARCHESAN (TATU)</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>A7FFF4C3-A8FA-4F96-841C-D5839B7DA92B</t>
+  </si>
+  <si>
     <t>AGRICOLA-MASSEY</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>8CCA2A1B-737E-481A-9CD3-F728223B44B1</t>
+  </si>
+  <si>
     <t>AGRICOLA-NEW HOOLAND</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>B6CAE4E3-9562-46E5-AB46-D25DA242A15F</t>
+  </si>
+  <si>
     <t>AGRICOLA-VALTRA</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>CF8931C2-B1ED-4BB3-AC74-A6A83E5ED28C</t>
+  </si>
+  <si>
     <t>AMARELA-CASE</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>A7690787-8DA9-47B0-A772-19A3A039F590</t>
+  </si>
+  <si>
     <t>AMARELA-CATERPILLAR</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>2CA5F7A3-627A-49D2-A308-C66F30DE3959</t>
+  </si>
+  <si>
     <t>AMARELA-DYNAPAC</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>7EB19327-E6C9-497C-B5CB-A6B29BF85893</t>
+  </si>
+  <si>
     <t>AMARELA-FIAT ALLIS</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>D3CF8BCB-2FD3-4986-85C4-E7A76BDE03A2</t>
+  </si>
+  <si>
     <t>AMARELA-JCB</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>848D7FD2-AAFE-4FB0-8194-6EE7AEF0F2E0</t>
+  </si>
+  <si>
     <t>AMARELA-KOMATSU</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
-    <t>AMARELA-TODOS</t>
-  </si>
-  <si>
-    <t>N</t>
+    <t>CFE0B1A5-5B1A-4F35-87CE-DAC04693FA40</t>
+  </si>
+  <si>
+    <t>AMARELA</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>7E7C89B0-8845-4A97-87DB-B23914368F09</t>
   </si>
   <si>
     <t>PESADA-IVECO</t>
@@ -139,76 +184,115 @@
     <t>N</t>
   </si>
   <si>
+    <t>52D670A0-9CB2-4F16-AC93-613D8CAD757A</t>
+  </si>
+  <si>
     <t>PESADA-FIAT</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>0E02FF74-13AD-4650-9782-5975591B8317</t>
+  </si>
+  <si>
     <t>PESADA-FORD</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>A82D2078-0A39-4A00-BF52-080107AF2C1E</t>
+  </si>
+  <si>
     <t>PESADA-GENERAL MOTORS  (CHEVROLET)</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>9F2FD525-DEB6-4FC6-ACE9-8C0AAE9DA3E1</t>
+  </si>
+  <si>
     <t>PESADA-GUERRA</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>FAC71209-6382-4AD7-B295-BAC5F8F64274</t>
+  </si>
+  <si>
     <t>PESADA-MERCEDES BENZ</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>049C1DAA-5D12-4E96-A705-0622AF21338D</t>
+  </si>
+  <si>
     <t>PESADA-RANDON</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>968FD0BE-6984-4C8C-BE13-47A01E600585</t>
+  </si>
+  <si>
     <t>PESADA-SCANIA</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>13676451-542E-4E96-AB49-E3015F477BA6</t>
+  </si>
+  <si>
     <t>PESADA-VOLKSWAGEN</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>226284CF-90F4-47BF-877A-3691702AB1C5</t>
+  </si>
+  <si>
     <t>PESADA-VOLVO</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>6447D833-BA0E-45E0-904F-825E89C830BC</t>
+  </si>
+  <si>
     <t>PESADA-TODOS</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
-    <t>LINHA UTILITÁRIO</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>LINHA LEVE</t>
-  </si>
-  <si>
-    <t>N</t>
+    <t>54528B77-72ED-4530-8404-5028D60E6DDD</t>
+  </si>
+  <si>
+    <t>LINHA UTILITARIO</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>C1B56547-9AB5-4DDD-90CF-882EED195A75</t>
+  </si>
+  <si>
+    <t>LEVE</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>BD2B44C2-4D71-4C88-B0C4-F5C65E9A2FF4</t>
   </si>
   <si>
     <t>FERRAMENTAS</t>
@@ -217,103 +301,133 @@
     <t>N</t>
   </si>
   <si>
+    <t>C09A5233-3E01-424E-905B-B72B75305EE6</t>
+  </si>
+  <si>
     <t>BOMBAS</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>B1B6865F-27EE-4294-9DFC-0658457D6227</t>
+  </si>
+  <si>
     <t>AGRICOLA-FORD</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>F95F8D9E-E716-4D14-9B8E-682697C100C5</t>
+  </si>
+  <si>
     <t>IMPLEMENTOS</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>86ECC386-79B9-4573-9AF7-A2D210F03770</t>
+  </si>
+  <si>
     <t>IMPLEMENTOS</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>C300AF45-53FA-43DD-9BC8-F85247B8343E</t>
+  </si>
+  <si>
     <t>MOTO</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>D299D55C-D876-44C1-8415-5C555A39709B</t>
+  </si>
+  <si>
     <t>OFICINA</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>71A9B3A0-7CCC-4923-8AA4-1B19813BF152</t>
+  </si>
+  <si>
     <t>AGRICOLA-LANDINI</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>B611496A-11A0-408E-9FEF-5C5C4898C300</t>
+  </si>
+  <si>
     <t>COLHEITADEIRA</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>F4AD9D6B-0B83-4060-AEDE-206338635438</t>
+  </si>
+  <si>
     <t>PLANTADEIRA</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>556440D2-5DEA-4D14-9FB3-F1EB52DE3C77</t>
+  </si>
+  <si>
     <t>PULVERIZADOR</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>B935172E-2244-419F-BB47-AAE4103ABD3E</t>
+  </si>
+  <si>
     <t>IMPLEMENTOS-KUHN</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>98D9C196-A3BD-4071-A166-1C8BE2171601</t>
+  </si>
+  <si>
     <t>AMARELA-MICHIGAN</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>A2ABC2B4-C73A-4897-963C-4D326420C071</t>
+  </si>
+  <si>
     <t>AMARELA-NEW HOOLAND</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
+    <t>4EE2CB78-BD95-4F94-B798-77D9EC925568</t>
+  </si>
+  <si>
     <t>PESADA- CARRETA</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
-    <t>AVIÃO-MOTO-LEVE-UTILITÁRIO-PESADO-AGRÍCOLA</t>
-  </si>
-  <si>
-    <t>MOTO-LEVE-UTILITÁRIO-PESADO-AGRICOLA</t>
-  </si>
-  <si>
-    <t>LEVE-UTILITÁRIO-PESADO-AGRICOLA</t>
-  </si>
-  <si>
-    <t>UTILITÁRIO-PESADO-AGRICOLA</t>
-  </si>
-  <si>
-    <t>PESADO-AGRICOLA</t>
+    <t>4C48D241-56D9-47CF-A6DE-888B644F7314</t>
   </si>
   <si>
     <t>STARA</t>
@@ -322,7 +436,142 @@
     <t>N</t>
   </si>
   <si>
-    <t>LEVE-UTILITÁRIO</t>
+    <t>62B34635-2318-455A-82E6-A0EB18B2BCE1</t>
+  </si>
+  <si>
+    <t>AGRICOLA - FENDT</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>865A8ADC-A675-4ADF-A41F-723EDF5616B6</t>
+  </si>
+  <si>
+    <t>AGRICOLA</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>7980524C-7196-41D2-8537-A53022C65E5A</t>
+  </si>
+  <si>
+    <t>FORA DE ESTRADA (LINHA AMARELA)</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>02E4CC08-10EE-48D0-95FC-4A965E429231</t>
+  </si>
+  <si>
+    <t>LEVE / PESADA / UTILITARIO</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>BD64BCD4-E67B-4333-BCC7-901756CF6DAF</t>
+  </si>
+  <si>
+    <t>LEVE / PESADA / UTILITARIO / AGRICOLA</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>F7A12F96-0A3E-40D1-9279-2BCF20676AF0</t>
+  </si>
+  <si>
+    <t>LEVE / UTILITARIO</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>7FAC28DF-EE6E-45B6-992E-7ADEE236CBBC</t>
+  </si>
+  <si>
+    <t>PESADA</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>C48F87F7-09D3-4049-BC96-AF5B98AB551F</t>
+  </si>
+  <si>
+    <t>PESADA / AGRICOLA</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>FD1AFE49-6ADD-4389-A42B-A72FAB2BD4D0</t>
+  </si>
+  <si>
+    <t>PESADA / UTILITARIO</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>74AD60F8-EC66-473C-AB5E-5D26DC4EACBC</t>
+  </si>
+  <si>
+    <t>AMARELA / AGRICOLA</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>F7A6F2F5-2FCB-462E-B79E-2DA64382DF75</t>
+  </si>
+  <si>
+    <t>GERAL</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>067A2D38-80FF-4282-828B-38495D38DD9B</t>
+  </si>
+  <si>
+    <t>AGRICOLA / UTILITARIO</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>4F6E24BE-1FEF-492E-827D-B71551AFCD50</t>
+  </si>
+  <si>
+    <t>LEVE / UTILITARIO / AGRICOLA / AMARELA / INDUST / PESADA</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>2CDF7794-DC4E-4F7C-8F27-A866B3CEFE18</t>
+  </si>
+  <si>
+    <t>LUBRIFICANTES</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>6F66DA60-244F-4A71-89C7-FA7CA4449265</t>
+  </si>
+  <si>
+    <t>LEVE- IMPORTADOS</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>8014075C-03EE-4321-8861-680C011D6905</t>
   </si>
 </sst>
 </file>
@@ -665,7 +914,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -693,553 +942,842 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>31</v>
       </c>
-      <c r="C16" t="s">
+      <c r="B32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="B33" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>33</v>
       </c>
-      <c r="C17" t="s">
+      <c r="B34" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B35" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" t="s">
+        <v>104</v>
+      </c>
+      <c r="D35" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B36" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B37" t="s">
+        <v>109</v>
+      </c>
+      <c r="C37" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="B38" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
         <v>41</v>
       </c>
-      <c r="C21" t="s">
+      <c r="B39" t="s">
+        <v>115</v>
+      </c>
+      <c r="C39" t="s">
+        <v>116</v>
+      </c>
+      <c r="D39" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
         <v>42</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="B40" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" t="s">
+        <v>119</v>
+      </c>
+      <c r="D40" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>43</v>
       </c>
-      <c r="C22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="B41" t="s">
+        <v>121</v>
+      </c>
+      <c r="C41" t="s">
+        <v>122</v>
+      </c>
+      <c r="D41" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
         <v>45</v>
       </c>
-      <c r="C23" t="s">
+      <c r="B42" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42" t="s">
+        <v>125</v>
+      </c>
+      <c r="D42" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
         <v>46</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="B43" t="s">
+        <v>127</v>
+      </c>
+      <c r="C43" t="s">
+        <v>128</v>
+      </c>
+      <c r="D43" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
         <v>47</v>
       </c>
-      <c r="C24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="B44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C44" t="s">
+        <v>131</v>
+      </c>
+      <c r="D44" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
         <v>49</v>
       </c>
-      <c r="C25" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="B45" t="s">
+        <v>133</v>
+      </c>
+      <c r="C45" t="s">
+        <v>134</v>
+      </c>
+      <c r="D45" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
         <v>51</v>
       </c>
-      <c r="C26" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="B46" t="s">
+        <v>136</v>
+      </c>
+      <c r="C46" t="s">
+        <v>137</v>
+      </c>
+      <c r="D46" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
         <v>53</v>
       </c>
-      <c r="C27" t="s">
+      <c r="B47" t="s">
+        <v>139</v>
+      </c>
+      <c r="C47" t="s">
+        <v>140</v>
+      </c>
+      <c r="D47" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
         <v>54</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="B48" t="s">
+        <v>142</v>
+      </c>
+      <c r="C48" t="s">
+        <v>143</v>
+      </c>
+      <c r="D48" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
         <v>55</v>
       </c>
-      <c r="C28" t="s">
+      <c r="B49" t="s">
+        <v>145</v>
+      </c>
+      <c r="C49" t="s">
+        <v>146</v>
+      </c>
+      <c r="D49" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
         <v>56</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="B50" t="s">
+        <v>148</v>
+      </c>
+      <c r="C50" t="s">
+        <v>149</v>
+      </c>
+      <c r="D50" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
         <v>57</v>
       </c>
-      <c r="C29" t="s">
+      <c r="B51" t="s">
+        <v>151</v>
+      </c>
+      <c r="C51" t="s">
+        <v>152</v>
+      </c>
+      <c r="D51" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
         <v>58</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="B52" t="s">
+        <v>154</v>
+      </c>
+      <c r="C52" t="s">
+        <v>155</v>
+      </c>
+      <c r="D52" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
         <v>59</v>
       </c>
-      <c r="C30" t="s">
+      <c r="B53" t="s">
+        <v>157</v>
+      </c>
+      <c r="C53" t="s">
+        <v>158</v>
+      </c>
+      <c r="D53" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="B54" t="s">
+        <v>160</v>
+      </c>
+      <c r="C54" t="s">
+        <v>161</v>
+      </c>
+      <c r="D54" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
         <v>61</v>
       </c>
-      <c r="C31" t="s">
+      <c r="B55" t="s">
+        <v>163</v>
+      </c>
+      <c r="C55" t="s">
+        <v>164</v>
+      </c>
+      <c r="D55" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
         <v>62</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="B56" t="s">
+        <v>166</v>
+      </c>
+      <c r="C56" t="s">
+        <v>167</v>
+      </c>
+      <c r="D56" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
         <v>63</v>
       </c>
-      <c r="C32" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="B57" t="s">
+        <v>169</v>
+      </c>
+      <c r="C57" t="s">
+        <v>170</v>
+      </c>
+      <c r="D57" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
         <v>65</v>
       </c>
-      <c r="C33" t="s">
+      <c r="B58" t="s">
+        <v>172</v>
+      </c>
+      <c r="C58" t="s">
+        <v>173</v>
+      </c>
+      <c r="D58" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
         <v>66</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>32</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="B59" t="s">
+        <v>175</v>
+      </c>
+      <c r="C59" t="s">
+        <v>176</v>
+      </c>
+      <c r="D59" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
         <v>67</v>
       </c>
-      <c r="C34" t="s">
+      <c r="B60" t="s">
+        <v>178</v>
+      </c>
+      <c r="C60" t="s">
+        <v>179</v>
+      </c>
+      <c r="D60" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
         <v>68</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>34</v>
-      </c>
-      <c r="B36" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>73</v>
-      </c>
-      <c r="C37" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>38</v>
-      </c>
-      <c r="B38" t="s">
-        <v>75</v>
-      </c>
-      <c r="C38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>40</v>
-      </c>
-      <c r="B39" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>41</v>
-      </c>
-      <c r="B40" t="s">
-        <v>79</v>
-      </c>
-      <c r="C40" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>42</v>
-      </c>
-      <c r="B41" t="s">
-        <v>81</v>
-      </c>
-      <c r="C41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>43</v>
-      </c>
-      <c r="B42" t="s">
-        <v>83</v>
-      </c>
-      <c r="C42" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>45</v>
-      </c>
-      <c r="B43" t="s">
-        <v>85</v>
-      </c>
-      <c r="C43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>46</v>
-      </c>
-      <c r="B44" t="s">
-        <v>87</v>
-      </c>
-      <c r="C44" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>47</v>
-      </c>
-      <c r="B45" t="s">
-        <v>89</v>
-      </c>
-      <c r="C45" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>49</v>
-      </c>
-      <c r="B46" t="s">
-        <v>91</v>
-      </c>
-      <c r="C46" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>51</v>
-      </c>
-      <c r="B47" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>52</v>
-      </c>
-      <c r="B48" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>53</v>
-      </c>
-      <c r="B49" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>54</v>
-      </c>
-      <c r="B50" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>55</v>
-      </c>
-      <c r="B51" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
-        <v>56</v>
-      </c>
-      <c r="B52" t="s">
-        <v>98</v>
-      </c>
-      <c r="C52" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>57</v>
-      </c>
-      <c r="B53" t="s">
-        <v>100</v>
+      <c r="B61" t="s">
+        <v>181</v>
+      </c>
+      <c r="C61" t="s">
+        <v>182</v>
+      </c>
+      <c r="D61" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>